<commit_message>
update work for word dict
</commit_message>
<xml_diff>
--- a/18_Natural_Processing/NIA_DICT/띄어쓰기 제발 되라되라되라.xlsx
+++ b/18_Natural_Processing/NIA_DICT/띄어쓰기 제발 되라되라되라.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="413">
   <si>
     <t>Raw Sent</t>
   </si>
@@ -31,165 +31,516 @@
     <t>수술 범위 조정을 위해 트렌델렌버그 (Trendelenberg) 자세를 5 분 동안 유지 및 고정하였다.</t>
   </si>
   <si>
+    <t>수술 범위 조정을 위해 트렌델렌버그</t>
+  </si>
+  <si>
+    <t>Trendelenberg</t>
+  </si>
+  <si>
     <t>흥미로운 점은 주기적인 요추 천자가 교통뇌수두증(Communicating hydroce-phalus)에서 단기적인 치료법이 될 수 있다.</t>
   </si>
   <si>
+    <t>교통뇌수두증</t>
+  </si>
+  <si>
+    <t>Communicating hydroce - phalus</t>
+  </si>
+  <si>
     <t>종괴의 효과나 협착으로 인하여 나타나고 되고, 병변 위치에 따라서, 척수내압 (Interspinal pressure)의 변화가 뇌내압에 강력하게 작용할 수 있다.</t>
   </si>
   <si>
+    <t>척수내압</t>
+  </si>
+  <si>
+    <t>Interspinal pressure</t>
+  </si>
+  <si>
     <t>소뇌편도헤르니아(Cerebellar ton-sillar herniation)의 위험을 일으킬 수 있다.</t>
   </si>
   <si>
+    <t>소뇌편도헤르니아</t>
+  </si>
+  <si>
+    <t>Cerebellar ton - sillar herniation</t>
+  </si>
+  <si>
     <t>따라서 비 교통 뇌수두증에서의 척추마취의 경우 뇌줄기헤르니아(Brain stem herniation)의 위험이 있다.</t>
   </si>
   <si>
+    <t>따라서 비 교통 뇌수두증에서의 척추마취의 경우 뇌줄기헤르니아</t>
+  </si>
+  <si>
+    <t>Brain stem herniation</t>
+  </si>
+  <si>
     <t>경막천자(Dural puncture)로 인한 헤르니아 위험이 낮을 뿐 아니라, 요추 복강 단락술 수술이 요추의 경막천자를 통해 뇌척수액을 누출시키는 것이다.</t>
   </si>
   <si>
+    <t>경막천자</t>
+  </si>
+  <si>
+    <t>Dural puncture</t>
+  </si>
+  <si>
     <t>하지만 요추 복강 단락술 수술을 하는 경우, 요추내 압력(Lumbar spinal canal pressure)이 급격히 증가할 수있다.</t>
   </si>
   <si>
+    <t>요추내 압력</t>
+  </si>
+  <si>
+    <t>Lumbar spinal canal pressure</t>
+  </si>
+  <si>
     <t>척수관류압(Spinal cord perfusion pressure)가 악화될 수 있어, 저혈압을 막기 위해서 수액 동시투여와 승압제를 사 용하는 것이 필요하다.</t>
   </si>
   <si>
+    <t>척수관류압</t>
+  </si>
+  <si>
+    <t>Spinal cord perfusion pressure</t>
+  </si>
+  <si>
     <t>비결핵항산균(nontuberculous mycobacteria)은 결핵 균과 나병균을 제외한 항산균을 말한다.</t>
   </si>
   <si>
+    <t>비결핵항산균</t>
+  </si>
+  <si>
+    <t>nontuberculous mycobacteria</t>
+  </si>
+  <si>
     <t>또한 출생 시 BCG (Bacille of Calmette and Guerin) 예방접종을 받았다.</t>
   </si>
   <si>
     <t>인후 도말 호흡기 바이러스 및 세균 중합효소연쇄반응(polymerase chain reaction) 검사는 음성이었다.</t>
   </si>
   <si>
+    <t>인후 도말 호흡기 바이러스 및 세균 중합효소연쇄반응</t>
+  </si>
+  <si>
+    <t>polymerase chain reaction</t>
+  </si>
+  <si>
     <t>객담에서의 항산균 도말 검사(acid-fast bacillus smear test)와 결핵균 중합효소연쇄 반응 검사도 모두 음성이었다.</t>
   </si>
   <si>
+    <t>말 검사</t>
+  </si>
+  <si>
+    <t>acid - fast bacillus smear test</t>
+  </si>
+  <si>
     <t>흉수의 아데노신탈아미노효소(ade- nosinedeaminase, ADA)는 127 U/L이었다.</t>
   </si>
   <si>
+    <t>아미노효소</t>
+  </si>
+  <si>
+    <t>ade - nosinedeaminase , ADA</t>
+  </si>
+  <si>
     <t>단순 흉부방사선 (chest X-ray) 검사에서 오른쪽 폐에 다량의 흉수가 관찰되었다</t>
   </si>
   <si>
+    <t>단순 흉부방사선</t>
+  </si>
+  <si>
+    <t>chest X - ray</t>
+  </si>
+  <si>
     <t>패혈증 치료를 위하여 항생제(piperacillin/tazobactam)와 다량의 수액을 투여하였다.</t>
   </si>
   <si>
+    <t>항생제</t>
+  </si>
+  <si>
+    <t>piperacillin / tazobactam</t>
+  </si>
+  <si>
     <t>이러한 과정에서 요로감염(urinary tract infec-tion)에 의한 패혈증(sepsis)도 동반되어 입원과 퇴원을 반복하는 등 전신 상태가 매우 불안정하였다.</t>
   </si>
   <si>
+    <t>요로감염</t>
+  </si>
+  <si>
+    <t>urinary tract infec - tion</t>
+  </si>
+  <si>
+    <t>패혈증</t>
+  </si>
+  <si>
+    <t>sepsis</t>
+  </si>
+  <si>
     <t>이 남성은 4년 전에 직장암(rectal cancer)을 진단받은 후 항암치료를 받아왔다.</t>
   </si>
   <si>
+    <t>직장암</t>
+  </si>
+  <si>
+    <t>rectal cancer</t>
+  </si>
+  <si>
     <t>간에서 일어나는 일차 대사작용(first-pass metabolism)과 뇌혈관 장벽(blood-brain barrier)을 모두 피할 수 있다.</t>
   </si>
   <si>
+    <t>간에서 일어나는 일차 대사작용</t>
+  </si>
+  <si>
+    <t>first - pass metabolism</t>
+  </si>
+  <si>
+    <t>대사작용</t>
+  </si>
+  <si>
+    <t>뇌혈관 장벽</t>
+  </si>
+  <si>
+    <t>blood - brain barrier</t>
+  </si>
+  <si>
     <t>후두마스크(laryngeal mask airway, LMA)는 응급 상황에서의 기도유지는 물론 전신마취시에 기관내삽관을 대신하여 많이 사용되고 있다.</t>
   </si>
   <si>
+    <t>후두마스크</t>
+  </si>
+  <si>
+    <t>laryngeal mask airway , LMA</t>
+  </si>
+  <si>
     <t>수술 전 검사상 심초음파 검사에서 경도의 이완기 기능이상(isolated diastolic dysfunction grade 1)을 보였다.</t>
   </si>
   <si>
+    <t>이상</t>
+  </si>
+  <si>
+    <t>isolated diastolic dysfunction grade 1</t>
+  </si>
+  <si>
     <t>특별한 문제없이 45분 동안 i-gel을 사용한 환자에서 혀 끝에 저린감 (numbness)이 발생하여 2주 후에 자연 회복된 경우가 있었다.</t>
   </si>
   <si>
+    <t>저린감</t>
+  </si>
+  <si>
+    <t>numbness</t>
+  </si>
+  <si>
     <t>본 증례의 경우와는 다르게 혀의 부음(swelling)이 동반된 보고들이있다.</t>
   </si>
   <si>
+    <t>혀의 부음</t>
+  </si>
+  <si>
+    <t>swelling</t>
+  </si>
+  <si>
     <t>드물지만 폐암환자에서 자가항체가 발생하여 부종양 신경학적 증후군(para- neoplastic neurologic syndrome)이 발생하기도 한다.</t>
   </si>
   <si>
+    <t>드물지만 폐암환자에서 자가항체가 발생하여 부종양 신경학적 증후군</t>
+  </si>
+  <si>
+    <t>para - neoplastic neurologic syndrome</t>
+  </si>
+  <si>
     <t>CT는 폐암의 진단에 있어 매우 중요한 영상진단 법이며, 폐암의 스크리닝 및 병기설정(staging)에도 유용하다.</t>
   </si>
   <si>
+    <t>병기설정</t>
+  </si>
+  <si>
+    <t>staging</t>
+  </si>
+  <si>
     <t>외상(trauma), 염증, 퇴행성 질환 등에서 위 양성이 보일 수있다.</t>
   </si>
   <si>
+    <t>외상</t>
+  </si>
+  <si>
+    <t>trauma</t>
+  </si>
+  <si>
     <t>일반적으로 기관지경의 직경은 6 mm가량이며 분절하기관지(subsegmental bronchi)까지 관찰 및 검체 획득이 가능하다.</t>
   </si>
   <si>
+    <t>분절하기관지</t>
+  </si>
+  <si>
+    <t>subsegmental bronchi</t>
+  </si>
+  <si>
     <t>기관지경으로 병변이 관찰되지 않는 경우 기관지 세척술 및 솔질(brushing)이 진단율 향상에 도움을 준다.</t>
   </si>
   <si>
+    <t>솔질</t>
+  </si>
+  <si>
+    <t>brushing</t>
+  </si>
+  <si>
     <t>또한 보이지 않는 말초병변의 경우 투시하 경기관지 조직검사(tranbronchial lung biopsy, TBLB)로 검체를 얻을 수 있다.</t>
   </si>
   <si>
+    <t>조직검사</t>
+  </si>
+  <si>
+    <t>tranbronchial lung biopsy , TBLB</t>
+  </si>
+  <si>
     <t>방사형 초음파 탐침(radial ultrasound probe)을 이용하여 말초병변의 조직을 채취하는 방법이다</t>
   </si>
   <si>
+    <t>방사형 초음파 탐침</t>
+  </si>
+  <si>
+    <t>radial ultrasound probe</t>
+  </si>
+  <si>
     <t>유전자 변화(genetic alterations)는 암의 개시, 성장, 진행의 중요한 기전이다.</t>
   </si>
   <si>
+    <t>유전자 변화</t>
+  </si>
+  <si>
+    <t>genetic alterations</t>
+  </si>
+  <si>
     <t>2개의 핵산길잡이(primer)를 이용하여 DNA를 증폭하여 검출하는 방법이다.</t>
   </si>
   <si>
+    <t>의 핵산길잡이</t>
+  </si>
+  <si>
+    <t>primer</t>
+  </si>
+  <si>
     <t>Sanger 염기서열 분석(sequencing)이 돌연변이를 검출하는 표준 방법이었으나 민감도가 충분히 높지 않고 노동과 시간이 많이 소비된다는 단점이 있다.</t>
   </si>
   <si>
+    <t>Sanger 염기서열 분석</t>
+  </si>
+  <si>
+    <t>sequencing</t>
+  </si>
+  <si>
     <t>최근 분자진단 기법의 발전으로 혈액, 흉수, 기관지폐포세척액 등 체액을 이용한 액체생검(liquid biopsy)이 임상에서 사용되고 있다.</t>
   </si>
   <si>
+    <t>액체생검</t>
+  </si>
+  <si>
+    <t>liquid biopsy</t>
+  </si>
+  <si>
     <t>분석 민감도 평가를 위해서 증폭산물 (amplicon) 염기서열 분석이 사용된다.</t>
   </si>
   <si>
+    <t>증폭산물</t>
+  </si>
+  <si>
+    <t>amplicon</t>
+  </si>
+  <si>
     <t>과거 순환 종양 세포(circulating tumor cell, CTC)에 대한 많은 연구가있었다.</t>
   </si>
   <si>
+    <t>과거 순환 종양 세포</t>
+  </si>
+  <si>
+    <t>circulating tumor cell , CTC</t>
+  </si>
+  <si>
     <t>첫 번째 수술은 요추 3번 에서 5번까지의 후방 감압술(Posterior decompression)이었다.</t>
   </si>
   <si>
+    <t>후방 감압술</t>
+  </si>
+  <si>
+    <t>Posterior decompression</t>
+  </si>
+  <si>
     <t>척추 수술과 같이 토니켓(tourniquet)을 사용할 수 없어 출혈을 조절할 수 없는 수술에 있어 출혈량이 증가할 경우 저혈량성 쇼크에 빠질 수 있다.</t>
   </si>
   <si>
+    <t>토니켓</t>
+  </si>
+  <si>
+    <t>tourniquet</t>
+  </si>
+  <si>
     <t>다(p-value  0. 006). 또한, 당 내성(Glucose tolerance)과 연관이 있는 OGTT 곡선</t>
   </si>
   <si>
+    <t>당 내성</t>
+  </si>
+  <si>
+    <t>Glucose tolerance</t>
+  </si>
+  <si>
     <t>전 세계 메타분석에서 체 질량지수(body mass index, BMI)와 말초혈관질환 위험 은 음의 상관관계가 보고되었다.</t>
   </si>
   <si>
+    <t>질량지수</t>
+  </si>
+  <si>
+    <t>body mass index , BMI</t>
+  </si>
+  <si>
     <t>적혈구 변형능(Erythrocyte deformability)은 적혈구의 형태 변화와 관련된 물리적 지표로서, 적혈구가 좁은 혈관을 매끄럽게 순환할 수 있도록 한다.</t>
   </si>
   <si>
+    <t>적혈구 변형능</t>
+  </si>
+  <si>
+    <t>Erythrocyte deformability</t>
+  </si>
+  <si>
     <t>미국당뇨병학회(ADA)의 옹호 활동은 당뇨병 연구 및 프로그램에 대한 정부 자금 지원, 건강 관리에 대한 접근 보장, 제 2 형 당뇨병 예방 촉진, 차별 퇴치 등을 망라한다.</t>
   </si>
   <si>
+    <t>미국당뇨병학회</t>
+  </si>
+  <si>
+    <t>ADA</t>
+  </si>
+  <si>
     <t>무과 (Cupressaceae)에 속한다.</t>
   </si>
   <si>
+    <t>무과</t>
+  </si>
+  <si>
+    <t>Cupressaceae</t>
+  </si>
+  <si>
     <t>RNA 실험용은 RNA  안정액 (RNAsolB)에 보관하여 일주일 안에 RNA를 추출하고, 나머지 부분은 액체질소로 급랭시켜 –70 ℃ 냉동고에 보관하 였다.</t>
   </si>
   <si>
+    <t>안정액</t>
+  </si>
+  <si>
+    <t>RNAsolB</t>
+  </si>
+  <si>
     <t>정상군  (Sham group)은 양쪽 슬관절강 내에 각각 주사용 생리식염 수 0. 1 ㎖을 주사하고 21일간 1일 1회 증류수를 경구투여 하 였다.</t>
   </si>
   <si>
+    <t>정상군</t>
+  </si>
+  <si>
+    <t>Sham group</t>
+  </si>
+  <si>
     <t>대조군 (Control group)은 양쪽 슬관절강 내에 각각  MIA 용액 0. 1 ㎖을 주사하여 골관절염을 유발시키면서 21일간 1일 1회 증류수를 경구투여 하였다.</t>
   </si>
   <si>
+    <t>대조군</t>
+  </si>
+  <si>
+    <t>Control group</t>
+  </si>
+  <si>
     <t>본 증례에서는 척추마취(Spinal anesthesia)를 통한 요추 복강 단락술을 받은 환자를 통해 마취적인 고찰을 하고자 한다.</t>
   </si>
   <si>
+    <t>척추마취</t>
+  </si>
+  <si>
+    <t>Spinal anesthesia</t>
+  </si>
+  <si>
     <t>뇌경색 및 신경아교증(Gliosis)의증 진단하에 종괴제거술 및 뇌생검 수술을 받기로 하였 다.</t>
   </si>
   <si>
+    <t>신경아교증</t>
+  </si>
+  <si>
+    <t>Gliosis</t>
+  </si>
+  <si>
     <t>뇌컴퓨터단층촬영에서 비교통성(non communicating) 유형의 뇌수두증(hydro-cephalus) 소견을 보여, 단락술 수술을 진행하기로 하였다.</t>
   </si>
   <si>
+    <t>비교통성</t>
+  </si>
+  <si>
+    <t>non communicating</t>
+  </si>
+  <si>
+    <t>뇌컴퓨터단층촬영에서 비교통성(non communicating) 유형의 뇌수두증</t>
+  </si>
+  <si>
+    <t>hydro - cephalus</t>
+  </si>
+  <si>
     <t>트리플힐릭스는 주로 지역단위에서 구현되며, 지식공간(Knowledge Spaces), 합의공간(ConsensusSpaces), 혁신공간(Innovation Spaces)으로 구성된3층위의 트리플힐릭스 공간체계가 형성되고 개별적인 트리플힐릭스 공간들이 상호작용하는 체계가 구축되었을 때, 지역혁신이 효과적으로 발현된다(Etzkowits, 2002; 이종호 외, 2009).트리플힐릭스 모델이 효과적으로 구축되기 위해서는 다음의 3가지 기본요소가 구축되어야 한다.</t>
   </si>
   <si>
+    <t>지식공간</t>
+  </si>
+  <si>
+    <t>Knowledge Spaces</t>
+  </si>
+  <si>
+    <t>혁신공간</t>
+  </si>
+  <si>
+    <t>Innovation Spaces</t>
+  </si>
+  <si>
+    <t>Knowledge</t>
+  </si>
+  <si>
+    <t>합의공간</t>
+  </si>
+  <si>
+    <t>ConsensusSpaces</t>
+  </si>
+  <si>
+    <t>Innovation</t>
+  </si>
+  <si>
     <t>적대적  M&amp;A를  일종의  시장  규율(market  discipline)로  보는  입장에서는  적대적  M&amp;A에  대한방어는  불가하다고  본다.</t>
   </si>
   <si>
+    <t>적대적  M&amp;A를  일종의  시장  규율</t>
+  </si>
+  <si>
+    <t>market discipline</t>
+  </si>
+  <si>
     <t>다만,  P2P  보험에  있어서  도덕적  해이  또는  Moral  Hazard로도  지칭되는보험사기를  법률상  어떻게  정의할지에  대한  검토가  필요하다.</t>
   </si>
   <si>
     <t>그  대신  그룹이  보험료를  설정하면  구성원은  해당  보험료로써  가상화폐를  에스크로우(Escrow)  계정으로써  디지털  지갑에  넣는다.</t>
   </si>
   <si>
+    <t>에스크로우</t>
+  </si>
+  <si>
+    <t>Escrow</t>
+  </si>
+  <si>
     <t>외국유한파트너쉽을 통한 국내투자의 경우 자금조달,  세제편의 등 여러 가지 사유로특수목적회사(SPC)를 이용하는 경우가 다수이다.</t>
   </si>
   <si>
+    <t>특수목적회사</t>
+  </si>
+  <si>
+    <t>SPC</t>
+  </si>
+  <si>
     <t>혼성단체(hybrid  entity)혼성비대칭 거래(hybrid  mismatch  arrangements)구나 2018년 5월 베이징에서 열린 ISO/TC 184 연례회의(Super Meeting)에서는 스마트 제조가 주요 화제였다.</t>
   </si>
   <si>
+    <t>혼성단체</t>
+  </si>
+  <si>
+    <t>hybrid entity</t>
+  </si>
+  <si>
     <t>이 행사에는 AVIC, SAC, WIZ, JLS 이노베이션스Innovations, 베이항 대학교Beihang University, 지멘스Siemens, 보잉Boeing 등 많은 산업 기관과 R&amp;D 기관의 참가자들이 참여했다.</t>
   </si>
   <si>
@@ -217,108 +568,423 @@
     <t>PwC  및 딜로이트(Deloitte)  등 대형 회계법인는 무엇인가?</t>
   </si>
   <si>
+    <t>딜로이트</t>
+  </si>
+  <si>
+    <t>Deloitte</t>
+  </si>
+  <si>
     <t>규제약물법 (controlled substances act)  에 규정된 마약 중범죄의 법정형(상한)을하향 조정하는 내용을 담고 있다.</t>
   </si>
   <si>
+    <t>규제약물법</t>
+  </si>
+  <si>
+    <t>controlled substances act</t>
+  </si>
+  <si>
     <t>그리스 로마 신화의 이카로스Icarus가 나무로 날개를 만들어 밀랍으로 깃털을 붙여 하늘을 날았던 그 순간부터 인류는 중력을 거스르고 자유롭게 날기 위한 기계와 장치를 설계하고 만들어왔다.</t>
   </si>
   <si>
     <t>동  쟁점과  관련하여  스페인  소재  방코  포풀라(Banco  Popular)  은행의  정리사례가  시사하는  바가  있어  살펴보고자  한다.</t>
   </si>
   <si>
+    <t>포풀라</t>
+  </si>
+  <si>
+    <t>Banco Popular</t>
+  </si>
+  <si>
     <t>영국  내에  본점을  운영하고  있는  은행에  대하여는  영란은행(BOE)및  건전성감독청(PRA)이  부실  정리를  관할하고  있다.</t>
   </si>
   <si>
+    <t>영란은행</t>
+  </si>
+  <si>
+    <t>BOE</t>
+  </si>
+  <si>
+    <t>건전성감독청</t>
+  </si>
+  <si>
+    <t>PRA</t>
+  </si>
+  <si>
     <t>핀테크란,  금융(finance)과 기술(technology)의 결합어로,  융과 IT의 융합을 통한 금융서비스 및 산업이다.</t>
   </si>
   <si>
+    <t>금융</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>기술</t>
+  </si>
+  <si>
+    <t>technology</t>
+  </si>
+  <si>
     <t>특히, 금융산업은 핀테크(Fintech) 기술의 발달로 다른 산업과의 융합이 활발하고 혁신의 속도가 매우빠릅니다.</t>
   </si>
   <si>
+    <t>핀테크</t>
+  </si>
+  <si>
+    <t>Fintech</t>
+  </si>
+  <si>
     <t>IT 新기술 발전이 산업간 ‧ 업종간의 경계를 허물어뜨리는 이른바 빅 블러(Big Blur)*를 가속화시킴에 따라 기존 경제 ․ 금융의 패러다임도 큰 변화를 맞이하고있습니다.</t>
   </si>
   <si>
+    <t>빅 블러</t>
+  </si>
+  <si>
+    <t>Big Blur</t>
+  </si>
+  <si>
     <t>(디지털 변혁)둘째, 4차 산업혁명의 도래와 함께 사물인터넷(IoT), 인공지능(AI) 및 빅테이터 기술이 디지털 변혁과혁신을 주도하고 있는 점에 주목할 필요가 있습니다.</t>
   </si>
   <si>
+    <t>사물인터넷</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>인공지능</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
     <t>IT 기술을 규제 준수에 활용하는 레그테크(RegTech)를 적극 활용하여 리스크요인들을 효과적이고 효율적으로 통제해 나가야 합니다.</t>
   </si>
   <si>
+    <t>레그테크</t>
+  </si>
+  <si>
+    <t>RegTech</t>
+  </si>
+  <si>
     <t>새로운  정부는  1958년  6월  3일의  헌법적  법률(loiconstitutionnelle)의 가결을 통해 즉시 일정한 조건하에 새로운 제도를 설계하는 권한을획득했다.</t>
   </si>
   <si>
+    <t>새로운  정부는  1958년  6월  3일의  헌법적  법률</t>
+  </si>
+  <si>
+    <t>loiconstitutionnelle</t>
+  </si>
+  <si>
     <t xml:space="preserve">부산방문을 마치고 귀국한 중국인들이 부산 관광에서 좋았던 느낌 등을 편리하게 달 수 있도록 우리나라의관광정보 시스템 이외에도 중국의 ‘큐큐(QQ)’를 비롯한 포털 시스템에 지속적으로 안내될 수 있도록 종합적으로 대응할 필요가 있을 것이다. </t>
   </si>
   <si>
+    <t>큐</t>
+  </si>
+  <si>
+    <t>QQ</t>
+  </si>
+  <si>
     <t>다음으로  소비자의  행동을  고관여(high  involvement),  저관여(low  involvement)로구분하여  소비자의  행동특성에  관한  연구를  제시하고  있다.</t>
   </si>
   <si>
+    <t>고관여</t>
+  </si>
+  <si>
+    <t>high involvement</t>
+  </si>
+  <si>
+    <t>저관여</t>
+  </si>
+  <si>
+    <t>low involvement</t>
+  </si>
+  <si>
     <t>Keywords: 중국인(Chinese), 관광객(Tourist), 행동특성(Behavior Characteristic),시장 세분화 (Market Segmentation), 단체관광(Group Tour),개별(FIT)</t>
   </si>
   <si>
+    <t>중국인</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>관광객</t>
+  </si>
+  <si>
+    <t>Tourist</t>
+  </si>
+  <si>
+    <t>특성</t>
+  </si>
+  <si>
+    <t>Behavior</t>
+  </si>
+  <si>
+    <t>세분화</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>관광</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>개별</t>
+  </si>
+  <si>
+    <t>FIT</t>
+  </si>
+  <si>
+    <t>행동특성</t>
+  </si>
+  <si>
+    <t>Behavior Characteristic</t>
+  </si>
+  <si>
+    <t>Keywords: 중국인(Chinese), 관광객(Tourist), 행동특성(Behavior Characteristic),시장 세분화</t>
+  </si>
+  <si>
+    <t>Market Segmentation</t>
+  </si>
+  <si>
+    <t>단체관광</t>
+  </si>
+  <si>
+    <t>Group Tour</t>
+  </si>
+  <si>
     <t>흔히 레디메이드는 파블로 피카소(Pablo Picasso)와 조르주 브라크(George  Braque)의 20기기 초반의 작품에서 그 기원을 찾는다.</t>
   </si>
   <si>
+    <t>흔히 레디메이드는 파블로 피카소</t>
+  </si>
+  <si>
+    <t>Pablo Picasso</t>
+  </si>
+  <si>
+    <t>흔히 레디메이드는 파블로 피카소(Pablo Picasso)와 조르주 브라크</t>
+  </si>
+  <si>
+    <t>George Braque</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 작품은  '차용미술의  어머니'라고  불리는  일레인  스터트밴트(ElaineSturtevant)에 의하여 다시 작품화된다.</t>
   </si>
   <si>
+    <t>밴트</t>
+  </si>
+  <si>
+    <t>ElaineSturtevant</t>
+  </si>
+  <si>
     <t>설치미술로 유명한 제프 쿤스(Jeff  Koons)는 차용행위로 인하여 여러 번 저작권 소송에 휘말렸다.</t>
   </si>
   <si>
+    <t>제프 쿤스</t>
+  </si>
+  <si>
+    <t>Jeff Koons</t>
+  </si>
+  <si>
     <t xml:space="preserve">당시  가장  유력한  피의자는  살인  전과가  있었던  크리스터  페터손(Christer  Petterson)이라는 사람이었는데 페터손은 가장 근거리에서 그 사건을 목격하였다. </t>
   </si>
   <si>
+    <t>당시  가장  유력한  피의자는  살인  전과가  있었던  크리스터  페터손</t>
+  </si>
+  <si>
+    <t>Christer Petterson</t>
+  </si>
+  <si>
     <t>2006년 작가 마르쿠스 앤데르손(Markus  Andersson)은 스톡홀름 현대미술관에서 전시회를 가진다.</t>
   </si>
   <si>
+    <t>르손</t>
+  </si>
+  <si>
+    <t>Markus Andersson</t>
+  </si>
+  <si>
     <t>IMF에서는  자본적정성(capital adequacy)에 대해그룹 차원의 자본 규제가 없는 것을 지적했다.</t>
   </si>
   <si>
+    <t>자본적정성</t>
+  </si>
+  <si>
+    <t>capital adequacy</t>
+  </si>
+  <si>
     <t>BSN(인도네시아 NSB)은 현재 표준화에서 새로운 진로를 개발하고 있으며, 이를 표준화 분석가(Analyst of Standardization)라고 명명했다.</t>
   </si>
   <si>
+    <t>BSN(인도네시아 NSB)은 현재 표준화에서 새로운 진로를 개발하고 있으며, 이를 표준화 분석가</t>
+  </si>
+  <si>
+    <t>Analyst of Standardization</t>
+  </si>
+  <si>
     <t>소프트스킬(soft skill)과 하드스킬(hard skill)이다.</t>
   </si>
   <si>
+    <t>소프트스킬</t>
+  </si>
+  <si>
+    <t>soft skill</t>
+  </si>
+  <si>
+    <t>하드스킬</t>
+  </si>
+  <si>
+    <t>hard skill</t>
+  </si>
+  <si>
     <t>정석적 지식(BOK, Body of Knowledge)은 "무엇을", "어떻게", "누가"의 관점에서 전문적인 실무가 요구되는 기술 및 태도를 정의한다.</t>
   </si>
   <si>
+    <t>정석적 지식</t>
+  </si>
+  <si>
+    <t>BOK , Body of Knowledge</t>
+  </si>
+  <si>
     <t>유엔 아시아 태평양 경제 사회 위원회(ESCAP)와 UNCTAD에서 10월 14일에 발행한 신규 보고서에 따르면, 아시아 태평양 지역에 적용된 관세는 지난 20년간 절반으로 줄었지만 국제무역에 영향을 미치는 관세 외 정책 규정은 유의하게 증가하였다.</t>
   </si>
   <si>
+    <t>유엔 아시아 태평양 경제 사회</t>
+  </si>
+  <si>
+    <t>ESCAP</t>
+  </si>
+  <si>
     <t>비관세조치의 국제 등급분류(ICNTM)의 목표는 신규 및 기존 조치의 국가간 공존성을 개선하도록 그러한 조치에 대한 정보와 설명을 제공하는 데에 있다.</t>
   </si>
   <si>
+    <t>비관세조치의 국제 등급분류</t>
+  </si>
+  <si>
+    <t>ICNTM</t>
+  </si>
+  <si>
     <t>UNCTAD의 무역분석정보시스템 (TRAINS) 내 NTM의 등급분류</t>
   </si>
   <si>
+    <t>UNCTAD의 무역분석정보시스템</t>
+  </si>
+  <si>
+    <t>TRAINS</t>
+  </si>
+  <si>
     <t>트위터(twitter)를 통해 IEC 고객서비스센터에 연락하세요.</t>
   </si>
   <si>
+    <t>트위터</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
+  <si>
     <t>저는 국가기술표준원(KATS)의 기술규제협력과 과장으로 있는 박재형입니다.</t>
   </si>
   <si>
+    <t>국가기술표준원</t>
+  </si>
+  <si>
+    <t>KATS</t>
+  </si>
+  <si>
     <t>ISO(국제표준화기구)는 국가 표준기관(ISO 회원기관)의 전 세계 연맹체이다.</t>
   </si>
   <si>
+    <t>ISO(국제표준화기구)는 국가 표준기관</t>
+  </si>
+  <si>
+    <t>ISO</t>
+  </si>
+  <si>
     <t>절대 GHG 배출량은 매스 스트림(mass stream), 예를 들어 연간 CO2e 톤(tCO2e/yr) 단위로 표시한다.</t>
   </si>
   <si>
+    <t>매스 스트림</t>
+  </si>
+  <si>
+    <t>mass stream</t>
+  </si>
+  <si>
+    <t>톤</t>
+  </si>
+  <si>
+    <t>tCO 2 e / yr</t>
+  </si>
+  <si>
     <t>따라서 입력 스트림(input stream)의 탄소 질량 유량을 출력 스트림(output stream)의 탄소 질량 유량과 비교해야 한다.</t>
   </si>
   <si>
+    <t>입력 스트림</t>
+  </si>
+  <si>
+    <t>input stream</t>
+  </si>
+  <si>
+    <t>출력 스트림</t>
+  </si>
+  <si>
+    <t>output stream</t>
+  </si>
+  <si>
     <t>ISO/TMBG란 ISO 기술관리이사회(TMB)에 보고된 그룹을 뜻한다.</t>
   </si>
   <si>
+    <t>ISO/TMBG란 ISO 기술관리이사회</t>
+  </si>
+  <si>
+    <t>TMB</t>
+  </si>
+  <si>
     <t>또한, UN 지속가능개발목표(SDG)에 따른 경제 개발, 사회적 진보 및 환경 보호에 기여할 것이다.</t>
   </si>
   <si>
+    <t>또한, UN 지속가능개발목표</t>
+  </si>
+  <si>
+    <t>SDG</t>
+  </si>
+  <si>
     <t>무역기술장벽(Technical Barrier to Trade, TBT) 조사 포인트를 강화하고 양질의 규제 관행 구현의 중요성과 기술 규제 근거로서의 표준 사용에 대한 규제 기관의 인식을 강화하여 TBT 관련 세계무역기구(WTO) 협정의 이행을 지원한다.</t>
   </si>
   <si>
+    <t>무역기술장벽</t>
+  </si>
+  <si>
+    <t>Technical Barrier to Trade , TBT</t>
+  </si>
+  <si>
+    <t>무역기술장벽(Technical Barrier to Trade, TBT) 조사 포인트를 강화하고 양질의 규제 관행 구</t>
+  </si>
+  <si>
+    <t>WTO</t>
+  </si>
+  <si>
     <t>앨런 울프(Alan Wolff) 세계무역기구(WTO) 사무차장은 올해 제네바에서 열린 총회에서 우리의 환영을 받은 참가자 중 하나였다.</t>
   </si>
   <si>
+    <t>앨런 울프</t>
+  </si>
+  <si>
+    <t>Alan Wolff</t>
+  </si>
+  <si>
+    <t>울프</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>세계무역기구</t>
+  </si>
+  <si>
     <t>지난 2년, ISOfocus가 2016년 사물인터넷(IoT)에 대한첫 보도를 발행한 후 매우 많은 일들이 있었다</t>
   </si>
   <si>
@@ -328,24 +994,75 @@
     <t>ISO는 WTO 무역촉진협정(TFA)의 이행과 함께 개발도상국의 ISO 회원 국가표준기구를 지원하기 위해 세계은행그룹과 제휴했다.</t>
   </si>
   <si>
+    <t>무역촉진협정</t>
+  </si>
+  <si>
+    <t>TFA</t>
+  </si>
+  <si>
     <t>사용하기 쉬운 프레임워크를 통해, 그 위치에 관계없이 캡티브(captive) 및 협력사 공장뿐 아니라 생산 시설 모두에 적용할 수 있다.</t>
   </si>
   <si>
+    <t>캡티브</t>
+  </si>
+  <si>
+    <t>captive</t>
+  </si>
+  <si>
     <t>년에는 유럽 개인정보보호법 (General Data Protection Regulations, GDPR)과 같은 법률이 목표로 하는 소비자 신뢰와 관련하여 발생된 명확한 위반으로 인해, 데이터 권리 및 프라이버시에 대한 소비자의 관심이 고조되었다.</t>
   </si>
   <si>
+    <t>년에는 유럽 개인정보보호법</t>
+  </si>
+  <si>
+    <t>General Data Protection Regulations , GDPR</t>
+  </si>
+  <si>
     <t>버트랜드 피카드(Bertrand Piccard),세계 최초 무동력 비행 항공기인 솔라 임펄스의 선구자</t>
   </si>
   <si>
+    <t>버트랜드</t>
+  </si>
+  <si>
+    <t>Bertrand Piccard</t>
+  </si>
+  <si>
     <t>제네바 재단(Fondation pour Genève)과 스위스 미션(Swiss Mission)이 협력한 덕분에, SDG 7(지속가능한 청정 에너지)와 SDG 13(기후 변화 대응)과 관련한 인포그래픽을 인쇄하여, 에너지 사용과 기후변화에 대처하는 ISO 표준의 역할을 가시화하였다.</t>
   </si>
   <si>
+    <t>제네바 재단</t>
+  </si>
+  <si>
+    <t>Fondation pour Genève</t>
+  </si>
+  <si>
+    <t>Fondation pour</t>
+  </si>
+  <si>
+    <t>스위스 미션</t>
+  </si>
+  <si>
+    <t>Swiss Mission</t>
+  </si>
+  <si>
     <t>이 센터는 어번 대학교(Auburn University), NASA, 제조 기술 혁신 조직인 EWI, 영국 기반의 제조 기술 센터 등을 한데 통합했습니다.</t>
   </si>
   <si>
+    <t>어번 대학교</t>
+  </si>
+  <si>
+    <t>Auburn University</t>
+  </si>
+  <si>
     <t>적층 제조(additive manufacturing) 기술(F42) 위원회의 새로운 표준은 고품질의 항공 부품, 의료 기기, 기타 부품 제조 시 3D 프린팅의 티타늄, 알루미늄 등 사용이 증가하고 있는 재료를 지원했습니다.표준은 기계 및 공정 적격화, 파우더 베드 퓨전 기술, 특성화 및 성능 이슈 등의 분야를 관장합니다.</t>
   </si>
   <si>
+    <t>적층 제조</t>
+  </si>
+  <si>
+    <t>additive manufacturing</t>
+  </si>
+  <si>
     <t>이벤트 주제로는 적층 제조(additive manufacturing), 건축 및 건설, 대마초, 국가 안보, 벽돌, 농약, 토양, 암석 등을 다루었습니다.</t>
   </si>
   <si>
@@ -355,36 +1072,132 @@
     <t>또한 친환경 공공조달(Green Public Procurement)에 듀라브로즈 개념을 도입하기 위한 지침도 마련될 것이다.</t>
   </si>
   <si>
+    <t>친환경 공공조달</t>
+  </si>
+  <si>
+    <t>Green Public Procurement</t>
+  </si>
+  <si>
     <t>저희 다우(Dow)에서 생각하는 표준’이란, 자원 효율성 면에서 개선 여부에 대한 시험과 평가뿐 아니라 상위 25%의 우수성 선점을 가능하게 하는 주요한 원리이자 결정적 성공 요인입니다.</t>
   </si>
   <si>
+    <t>다우</t>
+  </si>
+  <si>
+    <t>Dow</t>
+  </si>
+  <si>
     <t>지식 기반의 친환경 제품 사전 표준화(Knowledge Based Biobased Products’ PreStandardization, KBBPPS) 사업은 이러한 제품에 대한 친환경 내용물 결정과 생분해성 시험체계를 다룬다.</t>
   </si>
   <si>
+    <t>지식 기반의 친환경 제품 사전 표준화</t>
+  </si>
+  <si>
+    <t>Knowledge Based Biobased Products ’ PreStandardization , KBBPPS</t>
+  </si>
+  <si>
     <t>작게 보면, 행정정보공개 정책부터 데이터 민주주의가 시작되었고 오픈거번먼트(Open Government) 정책부터 본격화 되었다.</t>
   </si>
   <si>
+    <t>트</t>
+  </si>
+  <si>
+    <t>Open Government</t>
+  </si>
+  <si>
     <t>A열 트리플힐릭스는 주로 지역단위에서 구현되며, 지식공간(Knowledge Spaces), 합의공간(ConsensusSpaces), 혁신공간(Innovation Spaces)으로 구성된3층위의 트리플힐릭스 공간체계가 형성되고 개별적인 트리플힐릭스 공간들이 상호작용하는 체계가 구축되었을 때, 지역혁신이 효과적으로 발현된다(Etzkowits, 2002; 이종호 외, 2009).트리플힐릭스 모델이 효과적으로 구축되기 위해서는 다음의 3가지 기본요소가 구축되어야 한다.</t>
   </si>
   <si>
     <t>일관성 비율(CR)은 일관성 지수(Consistence Index:CI), 무작위 지수(Random Index: RI)의 상관식으로 이루어진다.</t>
   </si>
   <si>
+    <t>일관성 비율</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>일관성 지수</t>
+  </si>
+  <si>
+    <t>Consistence</t>
+  </si>
+  <si>
+    <t>Consistence Index : CI</t>
+  </si>
+  <si>
+    <t>무작위 지수</t>
+  </si>
+  <si>
+    <t>Random Index : RI</t>
+  </si>
+  <si>
     <t>또한 빅데이터 추출을 위한 특성 파악, 매시업 등 데이터전처리(data preprocessing)를 수행 중에 있다.</t>
   </si>
   <si>
+    <t>또한 빅데이터 추출을 위한 특성 파악, 매시업 등 데이터전처리</t>
+  </si>
+  <si>
+    <t>data preprocessing</t>
+  </si>
+  <si>
     <t>분석을 위한 코드는 R 재단(R foundation)에서 제작·배포하고 있는 무료 상용 프로그램인 R과 서포트 프로그램인 R-studio를 이용하여 작성되었으며, 구조방정식 모형의 적합성 검정은 결정계수(R²)와 적합도(Goodness of Fit, GoF)를 이용하였다.</t>
   </si>
   <si>
+    <t>재단</t>
+  </si>
+  <si>
+    <t>R foundation</t>
+  </si>
+  <si>
     <t>국내에ㅅ는 아직 증기압을 이용한 파암파쇄 시공 현장이 없는 관계로 일본 제조업체(Nippon Kokki ㈜)가 과거 많은 시공을 통하여 수립한 터널공사 적용 진동 추정식을 사용하였다.</t>
   </si>
   <si>
+    <t>국내에ㅅ는 아직 증기압을 이용한 파암파쇄 시공 현장이 없는 관계로 일본 제조업체</t>
+  </si>
+  <si>
+    <t>Nippon Kokki ㈜)</t>
+  </si>
+  <si>
     <t>통계적 신뢰도 해석에 많이 사용되는 수명분포는 노말(Normal), 지수(Exponential), 와이블(Weibull) 분포 등이다.</t>
   </si>
   <si>
+    <t>노말</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>말</t>
+  </si>
+  <si>
+    <t>지수</t>
+  </si>
+  <si>
+    <t>Exponential</t>
+  </si>
+  <si>
+    <t>와이블</t>
+  </si>
+  <si>
+    <t>Weibull</t>
+  </si>
+  <si>
     <t>전체 사고 중 911건이 건설업(S  )에서 발생했고, 그 중 207건이 물체를 연결/조립/설치/해체(T  )하던 중에 발생했다.</t>
   </si>
   <si>
+    <t>건이 건설업</t>
+  </si>
+  <si>
+    <t>S </t>
+  </si>
+  <si>
+    <t>해체</t>
+  </si>
+  <si>
+    <t>T </t>
+  </si>
+  <si>
     <t>배치 계층에서는 긴 주기(long-term) 데이터를 주기적으로 미리 처리하여 사용자의 요구에 따라 그 결과를 제공한다.</t>
   </si>
   <si>
@@ -394,16 +1207,52 @@
     <t>그 결과 의사결정나무(Decision Tree)기법의 AUC는 0.</t>
   </si>
   <si>
+    <t>그 결과 의사결정나무</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
     <t>먼저, 인간(Man)과 관련한 재해원인으로는 불안전한(unsafe) 행동과 오남용(misuse)을 들 수 있으며, 이에 따라 드론의 제어나 방전, 낙하나 드론을 사용한 공격, 도촬, 위협 등의 위험요인들이 발생하게 된다.</t>
   </si>
   <si>
+    <t>인간</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>남용</t>
+  </si>
+  <si>
+    <t>misuse</t>
+  </si>
+  <si>
     <t>본 환자의 경우, 보호자가 전신마취(general anesthesia)를 거부하여 신경외과 의사와 수술 및 마취 방법에 대하여 상의하였다.</t>
   </si>
   <si>
+    <t>전신마취</t>
+  </si>
+  <si>
+    <t>general anesthesia</t>
+  </si>
+  <si>
     <t>빠 른 생리식염수 투여를(rapid fluid administration) 하였 다.</t>
   </si>
   <si>
+    <t>생리식염수 투여</t>
+  </si>
+  <si>
+    <t>rapid fluid administration</t>
+  </si>
+  <si>
     <t>이 연구는 크레인의 조작장치 상의 휴먼에러 도 포함하고 있으나 설계, 제작, 보전, 운전, 폐기 등크레인과 관련된 전 수명주기(life cycle)적인 내용을 담고 있어 조작장치의 양립성 등 인간공학적 문제에 집중된 결과를 내지 못했다.</t>
+  </si>
+  <si>
+    <t>전 수명주기</t>
+  </si>
+  <si>
+    <t>life cycle</t>
   </si>
 </sst>
 </file>
@@ -735,7 +1584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -757,7 +1606,1845 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56" t="s">
+        <v>159</v>
+      </c>
+      <c r="C56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="B57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" t="s">
+        <v>163</v>
+      </c>
+      <c r="C60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>166</v>
+      </c>
+      <c r="B61" t="s">
+        <v>167</v>
+      </c>
+      <c r="C61" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>172</v>
+      </c>
+      <c r="B63" t="s">
+        <v>173</v>
+      </c>
+      <c r="C63" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="B68" t="s">
+        <v>196</v>
+      </c>
+      <c r="C68" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>198</v>
+      </c>
+      <c r="B69" t="s">
+        <v>199</v>
+      </c>
+      <c r="C69" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" t="s">
+        <v>201</v>
+      </c>
+      <c r="C70" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" t="s">
+        <v>201</v>
+      </c>
+      <c r="C72" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" t="s">
+        <v>204</v>
+      </c>
+      <c r="C73" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>209</v>
+      </c>
+      <c r="B75" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76" t="s">
+        <v>212</v>
+      </c>
+      <c r="C76" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77" t="s">
+        <v>215</v>
+      </c>
+      <c r="C77" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>217</v>
+      </c>
+      <c r="B78" t="s">
+        <v>218</v>
+      </c>
+      <c r="C78" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>220</v>
+      </c>
+      <c r="B79" t="s">
+        <v>221</v>
+      </c>
+      <c r="C79" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>223</v>
+      </c>
+      <c r="B80" t="s">
+        <v>224</v>
+      </c>
+      <c r="C80" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="B81" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>228</v>
+      </c>
+      <c r="B82" t="s">
+        <v>229</v>
+      </c>
+      <c r="C82" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="B83" t="s">
+        <v>231</v>
+      </c>
+      <c r="C83" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="B84" t="s">
+        <v>233</v>
+      </c>
+      <c r="C84" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="B85" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="B86" t="s">
+        <v>237</v>
+      </c>
+      <c r="C86" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="B87" t="s">
+        <v>239</v>
+      </c>
+      <c r="C87" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="B88" t="s">
+        <v>229</v>
+      </c>
+      <c r="C88" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="B89" t="s">
+        <v>231</v>
+      </c>
+      <c r="C89" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="B90" t="s">
+        <v>233</v>
+      </c>
+      <c r="C90" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="B91" t="s">
+        <v>235</v>
+      </c>
+      <c r="C91" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="B92" t="s">
+        <v>237</v>
+      </c>
+      <c r="C92" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="B93" t="s">
+        <v>239</v>
+      </c>
+      <c r="C93" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="B94" t="s">
+        <v>241</v>
+      </c>
+      <c r="C94" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="B95" t="s">
+        <v>243</v>
+      </c>
+      <c r="C95" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="B96" t="s">
+        <v>245</v>
+      </c>
+      <c r="C96" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="B97" t="s">
+        <v>241</v>
+      </c>
+      <c r="C97" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="B98" t="s">
+        <v>243</v>
+      </c>
+      <c r="C98" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="B99" t="s">
+        <v>245</v>
+      </c>
+      <c r="C99" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="B100" t="s">
+        <v>241</v>
+      </c>
+      <c r="C100" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="B101" t="s">
+        <v>243</v>
+      </c>
+      <c r="C101" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="B102" t="s">
+        <v>245</v>
+      </c>
+      <c r="C102" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="B103" t="s">
+        <v>229</v>
+      </c>
+      <c r="C103" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="B104" t="s">
+        <v>231</v>
+      </c>
+      <c r="C104" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="B105" t="s">
+        <v>233</v>
+      </c>
+      <c r="C105" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="B106" t="s">
+        <v>235</v>
+      </c>
+      <c r="C106" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="B107" t="s">
+        <v>237</v>
+      </c>
+      <c r="C107" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="B108" t="s">
+        <v>239</v>
+      </c>
+      <c r="C108" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>247</v>
+      </c>
+      <c r="B109" t="s">
+        <v>248</v>
+      </c>
+      <c r="C109" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="B110" t="s">
+        <v>250</v>
+      </c>
+      <c r="C110" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="B111" t="s">
+        <v>248</v>
+      </c>
+      <c r="C111" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="B112" t="s">
+        <v>250</v>
+      </c>
+      <c r="C112" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>252</v>
+      </c>
+      <c r="B113" t="s">
+        <v>253</v>
+      </c>
+      <c r="C113" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>255</v>
+      </c>
+      <c r="B114" t="s">
+        <v>256</v>
+      </c>
+      <c r="C114" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>258</v>
+      </c>
+      <c r="B115" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>261</v>
+      </c>
+      <c r="B116" t="s">
+        <v>262</v>
+      </c>
+      <c r="C116" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>264</v>
+      </c>
+      <c r="B117" t="s">
+        <v>265</v>
+      </c>
+      <c r="C117" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>267</v>
+      </c>
+      <c r="B118" t="s">
+        <v>268</v>
+      </c>
+      <c r="C118" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>270</v>
+      </c>
+      <c r="B119" t="s">
+        <v>271</v>
+      </c>
+      <c r="C119" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="B120" t="s">
+        <v>273</v>
+      </c>
+      <c r="C120" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="B121" t="s">
+        <v>271</v>
+      </c>
+      <c r="C121" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="B122" t="s">
+        <v>273</v>
+      </c>
+      <c r="C122" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>275</v>
+      </c>
+      <c r="B123" t="s">
+        <v>276</v>
+      </c>
+      <c r="C123" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>278</v>
+      </c>
+      <c r="B124" t="s">
+        <v>279</v>
+      </c>
+      <c r="C124" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>281</v>
+      </c>
+      <c r="B125" t="s">
+        <v>282</v>
+      </c>
+      <c r="C125" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>284</v>
+      </c>
+      <c r="B126" t="s">
+        <v>285</v>
+      </c>
+      <c r="C126" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>287</v>
+      </c>
+      <c r="B127" t="s">
+        <v>288</v>
+      </c>
+      <c r="C127" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>290</v>
+      </c>
+      <c r="B128" t="s">
+        <v>291</v>
+      </c>
+      <c r="C128" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>293</v>
+      </c>
+      <c r="B129" t="s">
+        <v>294</v>
+      </c>
+      <c r="C129" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>296</v>
+      </c>
+      <c r="B130" t="s">
+        <v>297</v>
+      </c>
+      <c r="C130" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="B131" t="s">
+        <v>299</v>
+      </c>
+      <c r="C131" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>301</v>
+      </c>
+      <c r="B132" t="s">
+        <v>302</v>
+      </c>
+      <c r="C132" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="B133" t="s">
+        <v>304</v>
+      </c>
+      <c r="C133" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="B134" t="s">
+        <v>302</v>
+      </c>
+      <c r="C134" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="B135" t="s">
+        <v>304</v>
+      </c>
+      <c r="C135" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>306</v>
+      </c>
+      <c r="B136" t="s">
+        <v>307</v>
+      </c>
+      <c r="C136" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>309</v>
+      </c>
+      <c r="B137" t="s">
+        <v>310</v>
+      </c>
+      <c r="C137" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>312</v>
+      </c>
+      <c r="B138" t="s">
+        <v>313</v>
+      </c>
+      <c r="C138" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="B139" t="s">
+        <v>315</v>
+      </c>
+      <c r="C139" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>317</v>
+      </c>
+      <c r="B140" t="s">
+        <v>318</v>
+      </c>
+      <c r="C140" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="B141" t="s">
+        <v>320</v>
+      </c>
+      <c r="C141" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="B142" t="s">
+        <v>322</v>
+      </c>
+      <c r="C142" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>323</v>
+      </c>
+      <c r="B143" t="s">
+        <v>210</v>
+      </c>
+      <c r="C143" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>324</v>
+      </c>
+      <c r="B144" t="s">
+        <v>210</v>
+      </c>
+      <c r="C144" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>325</v>
+      </c>
+      <c r="B145" t="s">
+        <v>326</v>
+      </c>
+      <c r="C145" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>328</v>
+      </c>
+      <c r="B146" t="s">
+        <v>329</v>
+      </c>
+      <c r="C146" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>331</v>
+      </c>
+      <c r="B147" t="s">
+        <v>332</v>
+      </c>
+      <c r="C147" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>334</v>
+      </c>
+      <c r="B148" t="s">
+        <v>335</v>
+      </c>
+      <c r="C148" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>337</v>
+      </c>
+      <c r="B149" t="s">
+        <v>338</v>
+      </c>
+      <c r="C149" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="B150" t="s">
+        <v>338</v>
+      </c>
+      <c r="C150" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="B151" t="s">
+        <v>341</v>
+      </c>
+      <c r="C151" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>343</v>
+      </c>
+      <c r="B152" t="s">
+        <v>344</v>
+      </c>
+      <c r="C152" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>346</v>
+      </c>
+      <c r="B153" t="s">
+        <v>347</v>
+      </c>
+      <c r="C153" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>349</v>
+      </c>
+      <c r="B154" t="s">
+        <v>347</v>
+      </c>
+      <c r="C154" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>351</v>
+      </c>
+      <c r="B155" t="s">
+        <v>352</v>
+      </c>
+      <c r="C155" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>354</v>
+      </c>
+      <c r="B156" t="s">
+        <v>355</v>
+      </c>
+      <c r="C156" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>357</v>
+      </c>
+      <c r="B157" t="s">
+        <v>358</v>
+      </c>
+      <c r="C157" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>360</v>
+      </c>
+      <c r="B158" t="s">
+        <v>361</v>
+      </c>
+      <c r="C158" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>363</v>
+      </c>
+      <c r="B159" t="s">
+        <v>154</v>
+      </c>
+      <c r="C159" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="B160" t="s">
+        <v>156</v>
+      </c>
+      <c r="C160" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="B161" t="s">
+        <v>154</v>
+      </c>
+      <c r="C161" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="B162" t="s">
+        <v>159</v>
+      </c>
+      <c r="C162" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="B163" t="s">
+        <v>156</v>
+      </c>
+      <c r="C163" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="B164" t="s">
+        <v>154</v>
+      </c>
+      <c r="C164" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="B165" t="s">
+        <v>156</v>
+      </c>
+      <c r="C165" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>364</v>
+      </c>
+      <c r="B166" t="s">
+        <v>365</v>
+      </c>
+      <c r="C166" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="B167" t="s">
+        <v>367</v>
+      </c>
+      <c r="C167" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="B168" t="s">
+        <v>367</v>
+      </c>
+      <c r="C168" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="B169" t="s">
+        <v>370</v>
+      </c>
+      <c r="C169" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
+        <v>372</v>
+      </c>
+      <c r="B170" t="s">
+        <v>373</v>
+      </c>
+      <c r="C170" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>375</v>
+      </c>
+      <c r="B171" t="s">
+        <v>376</v>
+      </c>
+      <c r="C171" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>378</v>
+      </c>
+      <c r="B172" t="s">
+        <v>379</v>
+      </c>
+      <c r="C172" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>381</v>
+      </c>
+      <c r="B173" t="s">
+        <v>382</v>
+      </c>
+      <c r="C173" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="B174" t="s">
+        <v>384</v>
+      </c>
+      <c r="C174" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="B175" t="s">
+        <v>385</v>
+      </c>
+      <c r="C175" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="B176" t="s">
+        <v>387</v>
+      </c>
+      <c r="C176" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
+        <v>389</v>
+      </c>
+      <c r="B177" t="s">
+        <v>390</v>
+      </c>
+      <c r="C177" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="B178" t="s">
+        <v>392</v>
+      </c>
+      <c r="C178" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="B179" t="s">
+        <v>390</v>
+      </c>
+      <c r="C179" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="B180" t="s">
+        <v>392</v>
+      </c>
+      <c r="C180" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
+        <v>395</v>
+      </c>
+      <c r="B181" t="s">
+        <v>361</v>
+      </c>
+      <c r="C181" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
+        <v>396</v>
+      </c>
+      <c r="B182" t="s">
+        <v>397</v>
+      </c>
+      <c r="C182" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>399</v>
+      </c>
+      <c r="B183" t="s">
+        <v>400</v>
+      </c>
+      <c r="C183" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="B184" t="s">
+        <v>402</v>
+      </c>
+      <c r="C184" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="B185" t="s">
+        <v>400</v>
+      </c>
+      <c r="C185" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="B186" t="s">
+        <v>402</v>
+      </c>
+      <c r="C186" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>404</v>
+      </c>
+      <c r="B187" t="s">
+        <v>405</v>
+      </c>
+      <c r="C187" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>407</v>
+      </c>
+      <c r="B188" t="s">
+        <v>408</v>
+      </c>
+      <c r="C188" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
+        <v>410</v>
+      </c>
+      <c r="B189" t="s">
+        <v>411</v>
+      </c>
+      <c r="C189" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
succed to find good quality of english ㅠㅠ
</commit_message>
<xml_diff>
--- a/18_Natural_Processing/NIA_DICT/띄어쓰기 제발 되라되라되라.xlsx
+++ b/18_Natural_Processing/NIA_DICT/띄어쓰기 제발 되라되라되라.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="420">
   <si>
     <t>Raw Sent</t>
   </si>
@@ -28,28 +28,28 @@
     <t>MOR</t>
   </si>
   <si>
+    <t>흥미로운 점은 주기적인 요추 천자가 교통뇌수두증(Communicating hydroce-phalus)에서 단기적인 치료법이 될 수 있다.</t>
+  </si>
+  <si>
+    <t>교통뇌수두증</t>
+  </si>
+  <si>
+    <t>Communicating hydroce - phalus</t>
+  </si>
+  <si>
     <t>수술 범위 조정을 위해 트렌델렌버그 (Trendelenberg) 자세를 5 분 동안 유지 및 고정하였다.</t>
   </si>
   <si>
-    <t xml:space="preserve">트렌델렌버그 </t>
+    <t>트렌델렌버그</t>
   </si>
   <si>
     <t>Trendelenberg</t>
   </si>
   <si>
-    <t>흥미로운 점은 주기적인 요추 천자가 교통뇌수두증(Communicating hydroce-phalus)에서 단기적인 치료법이 될 수 있다.</t>
-  </si>
-  <si>
-    <t>교통뇌수두증</t>
-  </si>
-  <si>
-    <t>Communicating hydroce - phalus</t>
-  </si>
-  <si>
     <t>종괴의 효과나 협착으로 인하여 나타나고 되고, 병변 위치에 따라서, 척수내압 (Interspinal pressure)의 변화가 뇌내압에 강력하게 작용할 수 있다.</t>
   </si>
   <si>
-    <t xml:space="preserve">척수내압 </t>
+    <t>척수내압</t>
   </si>
   <si>
     <t>Interspinal pressure</t>
@@ -85,7 +85,7 @@
     <t>하지만 요추 복강 단락술 수술을 하는 경우, 요추내 압력(Lumbar spinal canal pressure)이 급격히 증가할 수있다.</t>
   </si>
   <si>
-    <t>요추내 압력</t>
+    <t>요추내압력</t>
   </si>
   <si>
     <t>Lumbar spinal canal pressure</t>
@@ -115,7 +115,7 @@
     <t>인후 도말 호흡기 바이러스 및 세균 중합효소연쇄반응(polymerase chain reaction) 검사는 음성이었다.</t>
   </si>
   <si>
-    <t>세균 중합효소연쇄반응</t>
+    <t>세균중합효소연쇄반응</t>
   </si>
   <si>
     <t>polymerase chain reaction</t>
@@ -124,7 +124,7 @@
     <t>객담에서의 항산균 도말 검사(acid-fast bacillus smear test)와 결핵균 중합효소연쇄 반응 검사도 모두 음성이었다.</t>
   </si>
   <si>
-    <t>말 검사</t>
+    <t>말검사</t>
   </si>
   <si>
     <t>acid - fast bacillus smear test</t>
@@ -133,7 +133,7 @@
     <t>흉수의 아데노신탈아미노효소(ade- nosinedeaminase, ADA)는 127 U/L이었다.</t>
   </si>
   <si>
-    <t>아미노효소</t>
+    <t>아데노신탈아미노효소</t>
   </si>
   <si>
     <t>ade - nosinedeaminase , ADA</t>
@@ -142,7 +142,7 @@
     <t>단순 흉부방사선 (chest X-ray) 검사에서 오른쪽 폐에 다량의 흉수가 관찰되었다</t>
   </si>
   <si>
-    <t xml:space="preserve">단순 흉부방사선 </t>
+    <t>단순흉부방사선</t>
   </si>
   <si>
     <t>chest X - ray</t>
@@ -184,13 +184,13 @@
     <t>간에서 일어나는 일차 대사작용(first-pass metabolism)과 뇌혈관 장벽(blood-brain barrier)을 모두 피할 수 있다.</t>
   </si>
   <si>
-    <t>일차 대사작용</t>
+    <t>일차대사작용</t>
   </si>
   <si>
     <t>first - pass metabolism</t>
   </si>
   <si>
-    <t>뇌혈관 장벽</t>
+    <t>뇌혈관장벽</t>
   </si>
   <si>
     <t>blood - brain barrier</t>
@@ -208,7 +208,7 @@
     <t>수술 전 검사상 심초음파 검사에서 경도의 이완기 기능이상(isolated diastolic dysfunction grade 1)을 보였다.</t>
   </si>
   <si>
-    <t>이완기 기능이상</t>
+    <t>이완기기능이상</t>
   </si>
   <si>
     <t>isolated diastolic dysfunction grade 1</t>
@@ -217,7 +217,7 @@
     <t>특별한 문제없이 45분 동안 i-gel을 사용한 환자에서 혀 끝에 저린감 (numbness)이 발생하여 2주 후에 자연 회복된 경우가 있었다.</t>
   </si>
   <si>
-    <t xml:space="preserve">저린감 </t>
+    <t>저린감</t>
   </si>
   <si>
     <t>numbness</t>
@@ -226,7 +226,7 @@
     <t>본 증례의 경우와는 다르게 혀의 부음(swelling)이 동반된 보고들이있다.</t>
   </si>
   <si>
-    <t>혀의 부음</t>
+    <t>혀의부음</t>
   </si>
   <si>
     <t>swelling</t>
@@ -235,7 +235,7 @@
     <t>드물지만 폐암환자에서 자가항체가 발생하여 부종양 신경학적 증후군(para- neoplastic neurologic syndrome)이 발생하기도 한다.</t>
   </si>
   <si>
-    <t>부종양 신경학적 증후군</t>
+    <t>부종양신경학적증후군</t>
   </si>
   <si>
     <t>para - neoplastic neurologic syndrome</t>
@@ -289,7 +289,7 @@
     <t>방사형 초음파 탐침(radial ultrasound probe)을 이용하여 말초병변의 조직을 채취하는 방법이다</t>
   </si>
   <si>
-    <t>방사형 초음파 탐침</t>
+    <t>방사형초음파탐침</t>
   </si>
   <si>
     <t>radial ultrasound probe</t>
@@ -298,7 +298,7 @@
     <t>유전자 변화(genetic alterations)는 암의 개시, 성장, 진행의 중요한 기전이다.</t>
   </si>
   <si>
-    <t>유전자 변화</t>
+    <t>유전자변화</t>
   </si>
   <si>
     <t>genetic alterations</t>
@@ -307,7 +307,7 @@
     <t>2개의 핵산길잡이(primer)를 이용하여 DNA를 증폭하여 검출하는 방법이다.</t>
   </si>
   <si>
-    <t>의 핵산길잡이</t>
+    <t>의핵산길잡이</t>
   </si>
   <si>
     <t>primer</t>
@@ -316,7 +316,7 @@
     <t>Sanger 염기서열 분석(sequencing)이 돌연변이를 검출하는 표준 방법이었으나 민감도가 충분히 높지 않고 노동과 시간이 많이 소비된다는 단점이 있다.</t>
   </si>
   <si>
-    <t>염기서열 분석</t>
+    <t>염기서열분석</t>
   </si>
   <si>
     <t>sequencing</t>
@@ -334,7 +334,7 @@
     <t>분석 민감도 평가를 위해서 증폭산물 (amplicon) 염기서열 분석이 사용된다.</t>
   </si>
   <si>
-    <t xml:space="preserve">증폭산물 </t>
+    <t>증폭산물</t>
   </si>
   <si>
     <t>amplicon</t>
@@ -343,7 +343,7 @@
     <t>과거 순환 종양 세포(circulating tumor cell, CTC)에 대한 많은 연구가있었다.</t>
   </si>
   <si>
-    <t>과거 순환 종양 세포</t>
+    <t>과거순환종양세포</t>
   </si>
   <si>
     <t>circulating tumor cell , CTC</t>
@@ -352,7 +352,7 @@
     <t>첫 번째 수술은 요추 3번 에서 5번까지의 후방 감압술(Posterior decompression)이었다.</t>
   </si>
   <si>
-    <t>후방 감압술</t>
+    <t>후방감압술</t>
   </si>
   <si>
     <t>Posterior decompression</t>
@@ -370,7 +370,7 @@
     <t>다(p-value  0. 006). 또한, 당 내성(Glucose tolerance)과 연관이 있는 OGTT 곡선</t>
   </si>
   <si>
-    <t>당 내성</t>
+    <t>당내성</t>
   </si>
   <si>
     <t>Glucose tolerance</t>
@@ -388,7 +388,7 @@
     <t>적혈구 변형능(Erythrocyte deformability)은 적혈구의 형태 변화와 관련된 물리적 지표로서, 적혈구가 좁은 혈관을 매끄럽게 순환할 수 있도록 한다.</t>
   </si>
   <si>
-    <t>적혈구 변형능</t>
+    <t>적혈구변형능</t>
   </si>
   <si>
     <t>Erythrocyte deformability</t>
@@ -406,7 +406,7 @@
     <t>무과 (Cupressaceae)에 속한다.</t>
   </si>
   <si>
-    <t xml:space="preserve">무과 </t>
+    <t>무과</t>
   </si>
   <si>
     <t>Cupressaceae</t>
@@ -415,7 +415,7 @@
     <t>RNA 실험용은 RNA  안정액 (RNAsolB)에 보관하여 일주일 안에 RNA를 추출하고, 나머지 부분은 액체질소로 급랭시켜 –70 ℃ 냉동고에 보관하 였다.</t>
   </si>
   <si>
-    <t xml:space="preserve">안정액 </t>
+    <t>안정액</t>
   </si>
   <si>
     <t>RNAsolB</t>
@@ -424,7 +424,7 @@
     <t>정상군  (Sham group)은 양쪽 슬관절강 내에 각각 주사용 생리식염 수 0. 1 ㎖을 주사하고 21일간 1일 1회 증류수를 경구투여 하 였다.</t>
   </si>
   <si>
-    <t xml:space="preserve">정상군  </t>
+    <t>정상군</t>
   </si>
   <si>
     <t>Sham group</t>
@@ -433,7 +433,7 @@
     <t>대조군 (Control group)은 양쪽 슬관절강 내에 각각  MIA 용액 0. 1 ㎖을 주사하여 골관절염을 유발시키면서 21일간 1일 1회 증류수를 경구투여 하였다.</t>
   </si>
   <si>
-    <t xml:space="preserve">대조군 </t>
+    <t>대조군</t>
   </si>
   <si>
     <t>Control group</t>
@@ -466,7 +466,7 @@
     <t>non communicating</t>
   </si>
   <si>
-    <t>유형의 뇌수두증</t>
+    <t>유형의뇌수두증</t>
   </si>
   <si>
     <t>hydro - cephalus</t>
@@ -496,7 +496,7 @@
     <t>적대적  M&amp;A를  일종의  시장  규율(market  discipline)로  보는  입장에서는  적대적  M&amp;A에  대한방어는  불가하다고  본다.</t>
   </si>
   <si>
-    <t>일종의  시장  규율</t>
+    <t>일종의시장규율</t>
   </si>
   <si>
     <t>market discipline</t>
@@ -532,6 +532,9 @@
     <t>hybrid entity</t>
   </si>
   <si>
+    <t>혼성비대칭거래</t>
+  </si>
+  <si>
     <t>hybrid mismatch arrangements</t>
   </si>
   <si>
@@ -571,7 +574,7 @@
     <t>규제약물법 (controlled substances act)  에 규정된 마약 중범죄의 법정형(상한)을하향 조정하는 내용을 담고 있다.</t>
   </si>
   <si>
-    <t xml:space="preserve">규제약물법 </t>
+    <t>규제약물법</t>
   </si>
   <si>
     <t>controlled substances act</t>
@@ -631,7 +634,7 @@
     <t>IT 新기술 발전이 산업간 ‧ 업종간의 경계를 허물어뜨리는 이른바 빅 블러(Big Blur)*를 가속화시킴에 따라 기존 경제 ․ 금융의 패러다임도 큰 변화를 맞이하고있습니다.</t>
   </si>
   <si>
-    <t>빅 블러</t>
+    <t>빅블러</t>
   </si>
   <si>
     <t>Big Blur</t>
@@ -664,7 +667,7 @@
     <t>새로운  정부는  1958년  6월  3일의  헌법적  법률(loiconstitutionnelle)의 가결을 통해 즉시 일정한 조건하에 새로운 제도를 설계하는 권한을획득했다.</t>
   </si>
   <si>
-    <t>헌법적  법률</t>
+    <t>헌법적법률</t>
   </si>
   <si>
     <t>loiconstitutionnelle</t>
@@ -715,7 +718,7 @@
     <t>Behavior</t>
   </si>
   <si>
-    <t xml:space="preserve">세분화 </t>
+    <t>세분화</t>
   </si>
   <si>
     <t>Market</t>
@@ -739,7 +742,7 @@
     <t>Behavior Characteristic</t>
   </si>
   <si>
-    <t xml:space="preserve">시장 세분화 </t>
+    <t>시장세분화</t>
   </si>
   <si>
     <t>Market Segmentation</t>
@@ -754,13 +757,13 @@
     <t>흔히 레디메이드는 파블로 피카소(Pablo Picasso)와 조르주 브라크(George  Braque)의 20기기 초반의 작품에서 그 기원을 찾는다.</t>
   </si>
   <si>
-    <t>파블로 피카소</t>
+    <t>파블로피카소</t>
   </si>
   <si>
     <t>Pablo Picasso</t>
   </si>
   <si>
-    <t>조르주 브라크</t>
+    <t>조르주브라크</t>
   </si>
   <si>
     <t>George Braque</t>
@@ -778,7 +781,7 @@
     <t>설치미술로 유명한 제프 쿤스(Jeff  Koons)는 차용행위로 인하여 여러 번 저작권 소송에 휘말렸다.</t>
   </si>
   <si>
-    <t>제프 쿤스</t>
+    <t>제프쿤스</t>
   </si>
   <si>
     <t>Jeff Koons</t>
@@ -787,7 +790,7 @@
     <t xml:space="preserve">당시  가장  유력한  피의자는  살인  전과가  있었던  크리스터  페터손(Christer  Petterson)이라는 사람이었는데 페터손은 가장 근거리에서 그 사건을 목격하였다. </t>
   </si>
   <si>
-    <t>크리스터  페터손</t>
+    <t>크리스터페터손</t>
   </si>
   <si>
     <t>Christer Petterson</t>
@@ -796,7 +799,7 @@
     <t>2006년 작가 마르쿠스 앤데르손(Markus  Andersson)은 스톡홀름 현대미술관에서 전시회를 가진다.</t>
   </si>
   <si>
-    <t>르쿠스 앤데르손</t>
+    <t>르손</t>
   </si>
   <si>
     <t>Markus Andersson</t>
@@ -814,7 +817,7 @@
     <t>BSN(인도네시아 NSB)은 현재 표준화에서 새로운 진로를 개발하고 있으며, 이를 표준화 분석가(Analyst of Standardization)라고 명명했다.</t>
   </si>
   <si>
-    <t>표준화 분석가</t>
+    <t>표준화분석가</t>
   </si>
   <si>
     <t>Analyst of Standardization</t>
@@ -838,7 +841,7 @@
     <t>정석적 지식(BOK, Body of Knowledge)은 "무엇을", "어떻게", "누가"의 관점에서 전문적인 실무가 요구되는 기술 및 태도를 정의한다.</t>
   </si>
   <si>
-    <t>정석적 지식</t>
+    <t>정석적지식</t>
   </si>
   <si>
     <t>BOK , Body of Knowledge</t>
@@ -847,7 +850,7 @@
     <t>유엔 아시아 태평양 경제 사회 위원회(ESCAP)와 UNCTAD에서 10월 14일에 발행한 신규 보고서에 따르면, 아시아 태평양 지역에 적용된 관세는 지난 20년간 절반으로 줄었지만 국제무역에 영향을 미치는 관세 외 정책 규정은 유의하게 증가하였다.</t>
   </si>
   <si>
-    <t>태평양 경제 사회 위원회</t>
+    <t>태평양경제사회위원회</t>
   </si>
   <si>
     <t>ESCAP</t>
@@ -856,7 +859,7 @@
     <t>비관세조치의 국제 등급분류(ICNTM)의 목표는 신규 및 기존 조치의 국가간 공존성을 개선하도록 그러한 조치에 대한 정보와 설명을 제공하는 데에 있다.</t>
   </si>
   <si>
-    <t>국제 등급분류</t>
+    <t>국제등급분류</t>
   </si>
   <si>
     <t>ICNTM</t>
@@ -865,7 +868,7 @@
     <t>UNCTAD의 무역분석정보시스템 (TRAINS) 내 NTM의 등급분류</t>
   </si>
   <si>
-    <t xml:space="preserve">무역분석정보시스템 </t>
+    <t>무역분석정보시스템</t>
   </si>
   <si>
     <t>TRAINS</t>
@@ -892,7 +895,7 @@
     <t>ISO(국제표준화기구)는 국가 표준기관(ISO 회원기관)의 전 세계 연맹체이다.</t>
   </si>
   <si>
-    <t>국가 표준기관</t>
+    <t>국가표준기관</t>
   </si>
   <si>
     <t>ISO</t>
@@ -901,7 +904,7 @@
     <t>절대 GHG 배출량은 매스 스트림(mass stream), 예를 들어 연간 CO2e 톤(tCO2e/yr) 단위로 표시한다.</t>
   </si>
   <si>
-    <t>매스 스트림</t>
+    <t>매스스트림</t>
   </si>
   <si>
     <t>mass stream</t>
@@ -916,13 +919,13 @@
     <t>따라서 입력 스트림(input stream)의 탄소 질량 유량을 출력 스트림(output stream)의 탄소 질량 유량과 비교해야 한다.</t>
   </si>
   <si>
-    <t>입력 스트림</t>
+    <t>입력스트림</t>
   </si>
   <si>
     <t>input stream</t>
   </si>
   <si>
-    <t>출력 스트림</t>
+    <t>출력스트림</t>
   </si>
   <si>
     <t>output stream</t>
@@ -955,7 +958,7 @@
     <t>Technical Barrier to Trade , TBT</t>
   </si>
   <si>
-    <t>관행 구현의 중요성과 기술 규제 근거로서의 표준 사용에 대한 규제 기관의 인식을 강화하여 TBT 관련 세계무역기구</t>
+    <t>관련세계무역기구</t>
   </si>
   <si>
     <t>WTO</t>
@@ -964,7 +967,7 @@
     <t>앨런 울프(Alan Wolff) 세계무역기구(WTO) 사무차장은 올해 제네바에서 열린 총회에서 우리의 환영을 받은 참가자 중 하나였다.</t>
   </si>
   <si>
-    <t>앨런 울프</t>
+    <t>앨런울프</t>
   </si>
   <si>
     <t>Alan Wolff</t>
@@ -1006,7 +1009,7 @@
     <t>년에는 유럽 개인정보보호법 (General Data Protection Regulations, GDPR)과 같은 법률이 목표로 하는 소비자 신뢰와 관련하여 발생된 명확한 위반으로 인해, 데이터 권리 및 프라이버시에 대한 소비자의 관심이 고조되었다.</t>
   </si>
   <si>
-    <t xml:space="preserve">유럽 개인정보보호법 </t>
+    <t>유럽개인정보보호법</t>
   </si>
   <si>
     <t>General Data Protection Regulations , GDPR</t>
@@ -1015,7 +1018,7 @@
     <t>버트랜드 피카드(Bertrand Piccard),세계 최초 무동력 비행 항공기인 솔라 임펄스의 선구자</t>
   </si>
   <si>
-    <t>버트랜드 피카드</t>
+    <t>버트랜드피카드</t>
   </si>
   <si>
     <t>Bertrand Piccard</t>
@@ -1024,13 +1027,13 @@
     <t>제네바 재단(Fondation pour Genève)과 스위스 미션(Swiss Mission)이 협력한 덕분에, SDG 7(지속가능한 청정 에너지)와 SDG 13(기후 변화 대응)과 관련한 인포그래픽을 인쇄하여, 에너지 사용과 기후변화에 대처하는 ISO 표준의 역할을 가시화하였다.</t>
   </si>
   <si>
-    <t>제네바 재단</t>
+    <t>제네바재단</t>
   </si>
   <si>
     <t>Fondation pour Genève</t>
   </si>
   <si>
-    <t>스위스 미션</t>
+    <t>스위스미션</t>
   </si>
   <si>
     <t>Swiss Mission</t>
@@ -1039,7 +1042,7 @@
     <t>이 센터는 어번 대학교(Auburn University), NASA, 제조 기술 혁신 조직인 EWI, 영국 기반의 제조 기술 센터 등을 한데 통합했습니다.</t>
   </si>
   <si>
-    <t>어번 대학교</t>
+    <t>어번대학교</t>
   </si>
   <si>
     <t>Auburn University</t>
@@ -1048,7 +1051,7 @@
     <t>적층 제조(additive manufacturing) 기술(F42) 위원회의 새로운 표준은 고품질의 항공 부품, 의료 기기, 기타 부품 제조 시 3D 프린팅의 티타늄, 알루미늄 등 사용이 증가하고 있는 재료를 지원했습니다.표준은 기계 및 공정 적격화, 파우더 베드 퓨전 기술, 특성화 및 성능 이슈 등의 분야를 관장합니다.</t>
   </si>
   <si>
-    <t>적층 제조</t>
+    <t>적층제조</t>
   </si>
   <si>
     <t>additive manufacturing</t>
@@ -1066,7 +1069,7 @@
     <t>또한 친환경 공공조달(Green Public Procurement)에 듀라브로즈 개념을 도입하기 위한 지침도 마련될 것이다.</t>
   </si>
   <si>
-    <t>친환경 공공조달</t>
+    <t>친환경공공조달</t>
   </si>
   <si>
     <t>Green Public Procurement</t>
@@ -1084,7 +1087,7 @@
     <t>지식 기반의 친환경 제품 사전 표준화(Knowledge Based Biobased Products’ PreStandardization, KBBPPS) 사업은 이러한 제품에 대한 친환경 내용물 결정과 생분해성 시험체계를 다룬다.</t>
   </si>
   <si>
-    <t>친환경 제품 사전 표준화</t>
+    <t>친환경제품사전표준화</t>
   </si>
   <si>
     <t>Knowledge Based Biobased Products ’ PreStandardization , KBBPPS</t>
@@ -1105,19 +1108,19 @@
     <t>일관성 비율(CR)은 일관성 지수(Consistence Index:CI), 무작위 지수(Random Index: RI)의 상관식으로 이루어진다.</t>
   </si>
   <si>
-    <t>일관성 비율</t>
+    <t>일관성비율</t>
   </si>
   <si>
     <t>CR</t>
   </si>
   <si>
-    <t>일관성 지수</t>
+    <t>일관성지수</t>
   </si>
   <si>
     <t>Consistence</t>
   </si>
   <si>
-    <t>무작위 지수</t>
+    <t>무작위지수</t>
   </si>
   <si>
     <t>Random Index : RI</t>
@@ -1126,7 +1129,7 @@
     <t>또한 빅데이터 추출을 위한 특성 파악, 매시업 등 데이터전처리(data preprocessing)를 수행 중에 있다.</t>
   </si>
   <si>
-    <t>매시업 등 데이터전처리</t>
+    <t>매시업등데이터전처리</t>
   </si>
   <si>
     <t>data preprocessing</t>
@@ -1141,13 +1144,16 @@
     <t>R foundation</t>
   </si>
   <si>
+    <t>결정계수</t>
+  </si>
+  <si>
     <t>R ²)</t>
   </si>
   <si>
     <t>국내에ㅅ는 아직 증기압을 이용한 파암파쇄 시공 현장이 없는 관계로 일본 제조업체(Nippon Kokki ㈜)가 과거 많은 시공을 통하여 수립한 터널공사 적용 진동 추정식을 사용하였다.</t>
   </si>
   <si>
-    <t>일본 제조업체</t>
+    <t>일본제조업체</t>
   </si>
   <si>
     <t>Nippon Kokki ㈜)</t>
@@ -1177,7 +1183,7 @@
     <t>전체 사고 중 911건이 건설업(S  )에서 발생했고, 그 중 207건이 물체를 연결/조립/설치/해체(T  )하던 중에 발생했다.</t>
   </si>
   <si>
-    <t>건이 건설업</t>
+    <t>건설업</t>
   </si>
   <si>
     <t>S </t>
@@ -1198,7 +1204,7 @@
     <t>그 결과 의사결정나무(Decision Tree)기법의 AUC는 0.</t>
   </si>
   <si>
-    <t>그 결과 의사결정나무</t>
+    <t>그결과의사결정나무</t>
   </si>
   <si>
     <t>Decision Tree</t>
@@ -1231,7 +1237,7 @@
     <t>빠 른 생리식염수 투여를(rapid fluid administration) 하였 다.</t>
   </si>
   <si>
-    <t>생리식염수 투여를</t>
+    <t>생리식염수투여</t>
   </si>
   <si>
     <t>rapid fluid administration</t>
@@ -1240,7 +1246,7 @@
     <t>이 연구는 크레인의 조작장치 상의 휴먼에러 도 포함하고 있으나 설계, 제작, 보전, 운전, 폐기 등크레인과 관련된 전 수명주기(life cycle)적인 내용을 담고 있어 조작장치의 양립성 등 인간공학적 문제에 집중된 결과를 내지 못했다.</t>
   </si>
   <si>
-    <t>전 수명주기</t>
+    <t>전수명주기</t>
   </si>
   <si>
     <t>life cycle</t>
@@ -1264,7 +1270,7 @@
     <t>이에 따라 건설 프로젝트의 초기 단계에서 제한된 정보를 이용하여 공사비를 정확하게 추정 예측할 수 있는 방법에 대한 많은 연구가 이루어져 왔으며, 최근에는 딥러닝 등 머신러닝(Machine Learning)기술의 발전에 따라 공사비 예측 모델 개발에 이를 활용하는 연구가 매우 활발하게 이루어지고 있다.</t>
   </si>
   <si>
-    <t>딥러닝 등 머신러닝</t>
+    <t>딥러닝등머신러닝</t>
   </si>
   <si>
     <t>Machine Learning</t>
@@ -2233,708 +2239,711 @@
     </row>
     <row r="59" spans="1:3">
       <c r="B59" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C59" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B60" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C60" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B62" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C62" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B63" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="B64" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B65" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="B66" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C66" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B69" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C69" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="B70" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C70" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C71" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B72" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C72" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B73" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C73" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B74" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C74" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="B75" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C76" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="B77" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C77" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="B78" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C78" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="B79" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C79" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="B80" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C80" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="B81" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C81" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="B82" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C82" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="B83" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C83" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="B84" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C84" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B85" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C85" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="B86" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C86" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B87" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C87" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B89" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C89" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B90" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C90" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B91" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C91" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B92" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C92" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B93" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C93" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="B94" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C94" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B95" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C95" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B96" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C96" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B97" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C97" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B98" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C98" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B99" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C99" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B100" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B101" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C101" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B102" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C102" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="B103" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C103" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B104" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C104" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="B105" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C105" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B106" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C106" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B107" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C107" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B108" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C108" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="B109" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C109" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B110" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C110" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="B111" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C111" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="B112" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C112" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B113" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C113" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B114" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C114" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B115" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C115" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B116" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C116" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B117" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C117" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B118" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C118" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B119" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C119" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="B120" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C120" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B121" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C121" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B122" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C122" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="123" spans="1:3">
+      <c r="B123" t="s">
+        <v>200</v>
+      </c>
       <c r="C123" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B124" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C124" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B125" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C125" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B126" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C126" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B127" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C127" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B128" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C128" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B129" t="s">
         <v>153</v>
@@ -2961,217 +2970,220 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B132" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C132" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="B133" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C133" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="B134" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C134" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B135" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C135" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B136" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C136" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="137" spans="1:3">
+      <c r="B137" t="s">
+        <v>376</v>
+      </c>
       <c r="C137" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B138" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C138" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B139" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C139" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="B140" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C140" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="B141" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C141" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B142" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C142" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="B143" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C143" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B144" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C144" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B145" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C145" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B146" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C146" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="B147" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C147" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B148" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C148" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B149" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C149" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B150" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C150" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B151" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C151" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="B152" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C152" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B153" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C153" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>